<commit_message>
finish etude impact implementation plan and training plan
</commit_message>
<xml_diff>
--- a/Phase-1-preparation/Implementation plan/Implementation_plan.xlsx
+++ b/Phase-1-preparation/Implementation plan/Implementation_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelkonrath/Documents/Epitech/ProjetMSC1/Gotham/gotham_2020_20/Phase-1-preparation/Implementation plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC73461-97D3-F44A-A5BC-3D34D3ABBF7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A558A1C0-A15A-0245-8D17-4A5B430BF9D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{FB67EDAB-D69E-7F42-8F6B-C7628980C475}"/>
+    <workbookView xWindow="9840" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{FB67EDAB-D69E-7F42-8F6B-C7628980C475}"/>
   </bookViews>
   <sheets>
     <sheet name="Implementation plans" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
   <si>
     <t>Implementation  plans</t>
   </si>
@@ -205,6 +205,57 @@
   </si>
   <si>
     <t xml:space="preserve">HR department </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 - Change citizen's trashes </t>
+  </si>
+  <si>
+    <t>6 - public application for reporting incident and ask sanitation service</t>
+  </si>
+  <si>
+    <t>7 - Monthle reporting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discution with the municipality and a service provider </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor test in workhouse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">deployment of alert tool to get data from sensor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service provider/it department </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service provider </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deployment of the new trashes, th eold ones are sold by weight for recycling, and keep some undamager, just in case  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It departent referent / project manager </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srevice provider </t>
+  </si>
+  <si>
+    <t>Get data and analyze</t>
+  </si>
+  <si>
+    <t>take decision, to keep employees motivated and at the right level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chief departmenet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chief department </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5m, every start week, change a district trashes, and keep the rest of the weep to monitor and check malfunction </t>
+  </si>
+  <si>
+    <t>4d</t>
   </si>
 </sst>
 </file>
@@ -244,7 +295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,6 +332,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC9C1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8BFFDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF86BFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -294,11 +363,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -307,20 +373,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13079CE8-5A81-5043-852B-91A16C32A65E}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,347 +730,476 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="4" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C23" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="4" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="4" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="6" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+      <c r="B28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="11"/>
+      <c r="B29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A30" s="11"/>
+      <c r="B30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="12"/>
+      <c r="B32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="12"/>
+      <c r="B33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="12"/>
+      <c r="B34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="13"/>
+      <c r="B36" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A36"/>
     <mergeCell ref="A7:A15"/>
     <mergeCell ref="A16:A21"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A27:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>